<commit_message>
2 New Test Cases Passed
Tests Passed
</commit_message>
<xml_diff>
--- a/AutomationCucumber/src/test/resources/DataCucu.xlsx
+++ b/AutomationCucumber/src/test/resources/DataCucu.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git.Bertrand\AutomationCucumber\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6144"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6144" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="InvalidFields" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>Email</t>
   </si>
@@ -123,6 +125,18 @@
   </si>
   <si>
     <t>sadsada@hotmail.com</t>
+  </si>
+  <si>
+    <t>fgsdfgghfgh</t>
+  </si>
+  <si>
+    <t>sgfhsghsfgh</t>
+  </si>
+  <si>
+    <t>5465165</t>
+  </si>
+  <si>
+    <t>6344543</t>
   </si>
 </sst>
 </file>
@@ -237,7 +251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -247,12 +261,436 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="44">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -709,8 +1147,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:R4" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:R4" totalsRowShown="0" headerRowDxfId="43" headerRowBorderDxfId="42" tableBorderDxfId="41" totalsRowBorderDxfId="40">
   <autoFilter ref="A1:R4"/>
+  <tableColumns count="18">
+    <tableColumn id="1" name="Email" dataDxfId="39" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="2" name="FirstName" dataDxfId="38"/>
+    <tableColumn id="3" name="LastName" dataDxfId="37"/>
+    <tableColumn id="4" name="PasswordPI" dataDxfId="36"/>
+    <tableColumn id="5" name="days" dataDxfId="35"/>
+    <tableColumn id="6" name="months" dataDxfId="34"/>
+    <tableColumn id="7" name="years" dataDxfId="33"/>
+    <tableColumn id="8" name="Company" dataDxfId="32"/>
+    <tableColumn id="9" name="Address" dataDxfId="31"/>
+    <tableColumn id="10" name="Address2" dataDxfId="30"/>
+    <tableColumn id="11" name="City" dataDxfId="29"/>
+    <tableColumn id="12" name="State" dataDxfId="28"/>
+    <tableColumn id="13" name="ZipCode" dataDxfId="27"/>
+    <tableColumn id="14" name="Country" dataDxfId="26"/>
+    <tableColumn id="15" name="AdditionalInfo" dataDxfId="25"/>
+    <tableColumn id="16" name="Phone" dataDxfId="24"/>
+    <tableColumn id="17" name="MobilePhone" dataDxfId="23"/>
+    <tableColumn id="18" name="Alias" dataDxfId="22"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A1:R2" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="A1:R2"/>
   <tableColumns count="18">
     <tableColumn id="1" name="Email" dataDxfId="17" dataCellStyle="Hipervínculo"/>
     <tableColumn id="2" name="FirstName" dataDxfId="16"/>
@@ -1000,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,4 +1691,123 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test Case 5 passed
Check it out brodi
</commit_message>
<xml_diff>
--- a/AutomationCucumber/src/test/resources/DataCucu.xlsx
+++ b/AutomationCucumber/src/test/resources/DataCucu.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git.Bertrand\AutomationCucumber\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6144" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="6144" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="ProductName" sheetId="2" r:id="rId2"/>
     <sheet name="InvalidFields" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>Email</t>
   </si>
@@ -130,20 +130,23 @@
     <t>fgsdfgghfgh</t>
   </si>
   <si>
+    <t>gfhfdghfgh</t>
+  </si>
+  <si>
     <t>sgfhsghsfgh</t>
   </si>
   <si>
-    <t>5465165</t>
-  </si>
-  <si>
-    <t>6344543</t>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Faded Short Sleeve T-shirts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,16 +162,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -246,12 +269,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -264,6 +302,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -579,40 +619,50 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1695,12 +1745,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1709,8 +1775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1775,11 +1841,11 @@
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>36</v>
+      <c r="B2" s="5">
+        <v>546523165</v>
+      </c>
+      <c r="C2" s="5">
+        <v>652344543</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1795,9 +1861,11 @@
       </c>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
-      <c r="P2" s="7"/>
+      <c r="P2" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="Q2" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R2" s="6"/>
     </row>

</xml_diff>